<commit_message>
Se agrega lector de excel
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -19,19 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
-  <si>
-    <t>0116071817431743</t>
-  </si>
-  <si>
-    <t>0216071817431743</t>
-  </si>
-  <si>
-    <t>021607181852</t>
-  </si>
-  <si>
-    <t>0316071817431743</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Id_curso</t>
   </si>
@@ -85,6 +73,39 @@
   </si>
   <si>
     <t>d</t>
+  </si>
+  <si>
+    <t>00119.4Ā-9Ą1720;āċ071812ĆĖ47Đěē8č39Ġ902đĞģģ03ħĔĩīĤĂĤĞĔ3ĕ8ĶĥăĒĔĵķĹĲļĿ9ĔĆ04ĻĴ8Ęŋ4</t>
+  </si>
+  <si>
+    <t>Elemento</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Tal vez</t>
+  </si>
+  <si>
+    <t>Correo electrónico</t>
+  </si>
+  <si>
+    <t>mario</t>
+  </si>
+  <si>
+    <t>omar</t>
+  </si>
+  <si>
+    <t>fer</t>
+  </si>
+  <si>
+    <t>isma</t>
+  </si>
+  <si>
+    <t>Otra columna</t>
   </si>
 </sst>
 </file>
@@ -412,138 +433,182 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="82.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
+      <c r="H1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:10">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
         <v>23</v>
       </c>
-      <c r="G2" t="s">
-        <v>18</v>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2">
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3">
         <v>21</v>
       </c>
-      <c r="G3" t="s">
-        <v>19</v>
+      <c r="H3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3">
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4">
+        <v>56</v>
+      </c>
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>56</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4">
+        <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5">
         <v>9</v>
       </c>
-      <c r="E5" t="s">
-        <v>2</v>
-      </c>
-      <c r="F5">
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5">
         <v>89</v>
       </c>
-      <c r="G5" t="s">
-        <v>21</v>
+      <c r="H5" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="B8" s="2"/>
+    <row r="8" spans="1:10">
+      <c r="C8" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>